<commit_message>
Enhance the FileDataReader.readFromExcel method to be more user friendly
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/BookingTestData.xlsx
+++ b/src/test/resources/TestData/BookingTestData.xlsx
@@ -15,10 +15,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>Data Needed</t>
+    <t>Variable</t>
   </si>
   <si>
-    <t>Test Data</t>
+    <t>Data</t>
   </si>
   <si>
     <t>Email</t>
@@ -59,53 +59,110 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2560A7"/>
+        <bgColor rgb="FF2560A7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -343,914 +400,914 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>1.2345678E7</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>43784.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>43791.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="9"/>
     </row>
     <row r="11">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="9"/>
     </row>
     <row r="12">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
     </row>
     <row r="14">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
     </row>
     <row r="15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
     </row>
     <row r="16">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
     </row>
     <row r="19">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
     </row>
     <row r="20">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="9"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="9"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
+      <c r="A82" s="9"/>
+      <c r="B82" s="9"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="9"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
+      <c r="A88" s="9"/>
+      <c r="B88" s="9"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="9"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="9"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
+      <c r="A94" s="9"/>
+      <c r="B94" s="9"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
+      <c r="A95" s="9"/>
+      <c r="B95" s="9"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
+      <c r="A98" s="9"/>
+      <c r="B98" s="9"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
+      <c r="A99" s="9"/>
+      <c r="B99" s="9"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
+      <c r="A100" s="9"/>
+      <c r="B100" s="9"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
+      <c r="A102" s="9"/>
+      <c r="B102" s="9"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
+      <c r="A104" s="9"/>
+      <c r="B104" s="9"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
+      <c r="A105" s="9"/>
+      <c r="B105" s="9"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
+      <c r="A106" s="9"/>
+      <c r="B106" s="9"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
+      <c r="A107" s="9"/>
+      <c r="B107" s="9"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
+      <c r="A108" s="9"/>
+      <c r="B108" s="9"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
+      <c r="A110" s="9"/>
+      <c r="B110" s="9"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
+      <c r="A111" s="9"/>
+      <c r="B111" s="9"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
+      <c r="A112" s="9"/>
+      <c r="B112" s="9"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
+      <c r="A114" s="9"/>
+      <c r="B114" s="9"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
+      <c r="A115" s="9"/>
+      <c r="B115" s="9"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
+      <c r="A116" s="9"/>
+      <c r="B116" s="9"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
+      <c r="A118" s="9"/>
+      <c r="B118" s="9"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
+      <c r="A119" s="9"/>
+      <c r="B119" s="9"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
+      <c r="A120" s="9"/>
+      <c r="B120" s="9"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
+      <c r="A121" s="9"/>
+      <c r="B121" s="9"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
+      <c r="A122" s="9"/>
+      <c r="B122" s="9"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
+      <c r="A123" s="9"/>
+      <c r="B123" s="9"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
+      <c r="A124" s="9"/>
+      <c r="B124" s="9"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
+      <c r="A125" s="9"/>
+      <c r="B125" s="9"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
+      <c r="A126" s="9"/>
+      <c r="B126" s="9"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
+      <c r="A127" s="9"/>
+      <c r="B127" s="9"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
+      <c r="A128" s="9"/>
+      <c r="B128" s="9"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
+      <c r="A129" s="9"/>
+      <c r="B129" s="9"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
+      <c r="A130" s="9"/>
+      <c r="B130" s="9"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="1"/>
-      <c r="B131" s="1"/>
+      <c r="A131" s="9"/>
+      <c r="B131" s="9"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
+      <c r="A132" s="9"/>
+      <c r="B132" s="9"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="1"/>
-      <c r="B133" s="1"/>
+      <c r="A133" s="9"/>
+      <c r="B133" s="9"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="1"/>
-      <c r="B134" s="1"/>
+      <c r="A134" s="9"/>
+      <c r="B134" s="9"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="1"/>
-      <c r="B135" s="1"/>
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="1"/>
-      <c r="B136" s="1"/>
+      <c r="A136" s="9"/>
+      <c r="B136" s="9"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="1"/>
-      <c r="B137" s="1"/>
+      <c r="A137" s="9"/>
+      <c r="B137" s="9"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="1"/>
-      <c r="B138" s="1"/>
+      <c r="A138" s="9"/>
+      <c r="B138" s="9"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="1"/>
-      <c r="B139" s="1"/>
+      <c r="A139" s="9"/>
+      <c r="B139" s="9"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="1"/>
-      <c r="B140" s="1"/>
+      <c r="A140" s="9"/>
+      <c r="B140" s="9"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="1"/>
-      <c r="B141" s="1"/>
+      <c r="A141" s="9"/>
+      <c r="B141" s="9"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="1"/>
-      <c r="B142" s="1"/>
+      <c r="A142" s="9"/>
+      <c r="B142" s="9"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="1"/>
-      <c r="B143" s="1"/>
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
+      <c r="A144" s="9"/>
+      <c r="B144" s="9"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="1"/>
-      <c r="B145" s="1"/>
+      <c r="A145" s="9"/>
+      <c r="B145" s="9"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="1"/>
-      <c r="B146" s="1"/>
+      <c r="A146" s="9"/>
+      <c r="B146" s="9"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="1"/>
-      <c r="B147" s="1"/>
+      <c r="A147" s="9"/>
+      <c r="B147" s="9"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="1"/>
-      <c r="B148" s="1"/>
+      <c r="A148" s="9"/>
+      <c r="B148" s="9"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="1"/>
-      <c r="B149" s="1"/>
+      <c r="A149" s="9"/>
+      <c r="B149" s="9"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="1"/>
-      <c r="B150" s="1"/>
+      <c r="A150" s="9"/>
+      <c r="B150" s="9"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="1"/>
-      <c r="B151" s="1"/>
+      <c r="A151" s="9"/>
+      <c r="B151" s="9"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
+      <c r="A152" s="9"/>
+      <c r="B152" s="9"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
+      <c r="A153" s="9"/>
+      <c r="B153" s="9"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="1"/>
-      <c r="B154" s="1"/>
+      <c r="A154" s="9"/>
+      <c r="B154" s="9"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="1"/>
-      <c r="B155" s="1"/>
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
+      <c r="A156" s="9"/>
+      <c r="B156" s="9"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="1"/>
-      <c r="B157" s="1"/>
+      <c r="A157" s="9"/>
+      <c r="B157" s="9"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="1"/>
-      <c r="B158" s="1"/>
+      <c r="A158" s="9"/>
+      <c r="B158" s="9"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
+      <c r="A159" s="9"/>
+      <c r="B159" s="9"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="1"/>
-      <c r="B160" s="1"/>
+      <c r="A160" s="9"/>
+      <c r="B160" s="9"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="1"/>
-      <c r="B161" s="1"/>
+      <c r="A161" s="9"/>
+      <c r="B161" s="9"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="1"/>
-      <c r="B162" s="1"/>
+      <c r="A162" s="9"/>
+      <c r="B162" s="9"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="1"/>
-      <c r="B163" s="1"/>
+      <c r="A163" s="9"/>
+      <c r="B163" s="9"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="1"/>
-      <c r="B164" s="1"/>
+      <c r="A164" s="9"/>
+      <c r="B164" s="9"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="1"/>
-      <c r="B165" s="1"/>
+      <c r="A165" s="9"/>
+      <c r="B165" s="9"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="1"/>
-      <c r="B166" s="1"/>
+      <c r="A166" s="9"/>
+      <c r="B166" s="9"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="1"/>
-      <c r="B167" s="1"/>
+      <c r="A167" s="9"/>
+      <c r="B167" s="9"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="1"/>
-      <c r="B168" s="1"/>
+      <c r="A168" s="9"/>
+      <c r="B168" s="9"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="1"/>
-      <c r="B169" s="1"/>
+      <c r="A169" s="9"/>
+      <c r="B169" s="9"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="1"/>
-      <c r="B170" s="1"/>
+      <c r="A170" s="9"/>
+      <c r="B170" s="9"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="1"/>
-      <c r="B171" s="1"/>
+      <c r="A171" s="9"/>
+      <c r="B171" s="9"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="1"/>
-      <c r="B172" s="1"/>
+      <c r="A172" s="9"/>
+      <c r="B172" s="9"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="1"/>
-      <c r="B173" s="1"/>
+      <c r="A173" s="9"/>
+      <c r="B173" s="9"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="1"/>
-      <c r="B174" s="1"/>
+      <c r="A174" s="9"/>
+      <c r="B174" s="9"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="1"/>
-      <c r="B175" s="1"/>
+      <c r="A175" s="9"/>
+      <c r="B175" s="9"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="1"/>
-      <c r="B176" s="1"/>
+      <c r="A176" s="9"/>
+      <c r="B176" s="9"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="1"/>
-      <c r="B177" s="1"/>
+      <c r="A177" s="9"/>
+      <c r="B177" s="9"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="1"/>
-      <c r="B178" s="1"/>
+      <c r="A178" s="9"/>
+      <c r="B178" s="9"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="1"/>
-      <c r="B179" s="1"/>
+      <c r="A179" s="9"/>
+      <c r="B179" s="9"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="1"/>
-      <c r="B180" s="1"/>
+      <c r="A180" s="9"/>
+      <c r="B180" s="9"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="1"/>
-      <c r="B181" s="1"/>
+      <c r="A181" s="9"/>
+      <c r="B181" s="9"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="1"/>
-      <c r="B182" s="1"/>
+      <c r="A182" s="9"/>
+      <c r="B182" s="9"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="1"/>
-      <c r="B183" s="1"/>
+      <c r="A183" s="9"/>
+      <c r="B183" s="9"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="1"/>
-      <c r="B184" s="1"/>
+      <c r="A184" s="9"/>
+      <c r="B184" s="9"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="1"/>
-      <c r="B185" s="1"/>
+      <c r="A185" s="9"/>
+      <c r="B185" s="9"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="1"/>
-      <c r="B186" s="1"/>
+      <c r="A186" s="9"/>
+      <c r="B186" s="9"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="1"/>
-      <c r="B187" s="1"/>
+      <c r="A187" s="9"/>
+      <c r="B187" s="9"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="1"/>
-      <c r="B188" s="1"/>
+      <c r="A188" s="9"/>
+      <c r="B188" s="9"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="1"/>
-      <c r="B189" s="1"/>
+      <c r="A189" s="9"/>
+      <c r="B189" s="9"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="1"/>
-      <c r="B190" s="1"/>
+      <c r="A190" s="9"/>
+      <c r="B190" s="9"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="1"/>
-      <c r="B191" s="1"/>
+      <c r="A191" s="9"/>
+      <c r="B191" s="9"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="1"/>
-      <c r="B192" s="1"/>
+      <c r="A192" s="9"/>
+      <c r="B192" s="9"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="1"/>
-      <c r="B193" s="1"/>
+      <c r="A193" s="9"/>
+      <c r="B193" s="9"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="1"/>
-      <c r="B194" s="1"/>
+      <c r="A194" s="9"/>
+      <c r="B194" s="9"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="1"/>
-      <c r="B195" s="1"/>
+      <c r="A195" s="9"/>
+      <c r="B195" s="9"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="1"/>
-      <c r="B196" s="1"/>
+      <c r="A196" s="9"/>
+      <c r="B196" s="9"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="1"/>
-      <c r="B197" s="1"/>
+      <c r="A197" s="9"/>
+      <c r="B197" s="9"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="1"/>
-      <c r="B198" s="1"/>
+      <c r="A198" s="9"/>
+      <c r="B198" s="9"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="1"/>
-      <c r="B199" s="1"/>
+      <c r="A199" s="9"/>
+      <c r="B199" s="9"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="1"/>
-      <c r="B200" s="1"/>
+      <c r="A200" s="9"/>
+      <c r="B200" s="9"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="1"/>
-      <c r="B201" s="1"/>
+      <c r="A201" s="9"/>
+      <c r="B201" s="9"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="1"/>
-      <c r="B202" s="1"/>
+      <c r="A202" s="9"/>
+      <c r="B202" s="9"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="1"/>
-      <c r="B203" s="1"/>
+      <c r="A203" s="9"/>
+      <c r="B203" s="9"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="1"/>
-      <c r="B204" s="1"/>
+      <c r="A204" s="9"/>
+      <c r="B204" s="9"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="1"/>
-      <c r="B205" s="1"/>
+      <c r="A205" s="9"/>
+      <c r="B205" s="9"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="1"/>
-      <c r="B206" s="1"/>
+      <c r="A206" s="9"/>
+      <c r="B206" s="9"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="1"/>
-      <c r="B207" s="1"/>
+      <c r="A207" s="9"/>
+      <c r="B207" s="9"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="1"/>
-      <c r="B208" s="1"/>
+      <c r="A208" s="9"/>
+      <c r="B208" s="9"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="1"/>
-      <c r="B209" s="1"/>
+      <c r="A209" s="9"/>
+      <c r="B209" s="9"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="1"/>
-      <c r="B210" s="1"/>
+      <c r="A210" s="9"/>
+      <c r="B210" s="9"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="1"/>
-      <c r="B211" s="1"/>
+      <c r="A211" s="9"/>
+      <c r="B211" s="9"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="1"/>
-      <c r="B212" s="1"/>
+      <c r="A212" s="9"/>
+      <c r="B212" s="9"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="1"/>
-      <c r="B213" s="1"/>
+      <c r="A213" s="9"/>
+      <c r="B213" s="9"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="1"/>
-      <c r="B214" s="1"/>
+      <c r="A214" s="9"/>
+      <c r="B214" s="9"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="1"/>
-      <c r="B215" s="1"/>
+      <c r="A215" s="9"/>
+      <c r="B215" s="9"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="1"/>
-      <c r="B216" s="1"/>
+      <c r="A216" s="9"/>
+      <c r="B216" s="9"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="1"/>
-      <c r="B217" s="1"/>
+      <c r="A217" s="9"/>
+      <c r="B217" s="9"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="1"/>
-      <c r="B218" s="1"/>
+      <c r="A218" s="9"/>
+      <c r="B218" s="9"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="1"/>
-      <c r="B219" s="1"/>
+      <c r="A219" s="9"/>
+      <c r="B219" s="9"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="1"/>
-      <c r="B220" s="1"/>
+      <c r="A220" s="9"/>
+      <c r="B220" s="9"/>
     </row>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>

</xml_diff>